<commit_message>
#457, add WHO's COVID-19 product list
</commit_message>
<xml_diff>
--- a/pim/src/PcmtCustomDatasetBundle/Resources/fixtures/pcmt_global/import_files/2020-03-29/11_datagrid_view.xlsx
+++ b/pim/src/PcmtCustomDatasetBundle/Resources/fixtures/pcmt_global/import_files/2020-03-29/11_datagrid_view.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="39">
   <si>
     <t xml:space="preserve">label</t>
   </si>
@@ -49,7 +49,7 @@
     <t xml:space="preserve">product-grid</t>
   </si>
   <si>
-    <t xml:space="preserve">i=1&amp;p=25&amp;s%5BL3%5D=-1&amp;f%5Bfamily%5D%5Bvalue%5D%5B%5D=RH_PRODUCTS_TRADEITEMS_VARIANTS&amp;f%5Bfamily%5D%5Btype%5D=in&amp;f%5Bcategory%5D%5Bvalue%5D%5BtreeId%5D=8&amp;f%5Bcategory%5D%5Bvalue%5D%5BcategoryId%5D=0&amp;f%5Bcategory%5D%5Btype%5D=1&amp;t=product-grid</t>
+    <t xml:space="preserve">i=2&amp;p=25&amp;s%5BL3%5D=-1&amp;f%5Bscope%5D%5Bvalue%5D=PRODUCT_CATALOG&amp;f%5Bcategory%5D%5Bvalue%5D%5BtreeId%5D=1&amp;f%5Bcategory%5D%5Bvalue%5D%5BcategoryId%5D=5&amp;f%5Bcategory%5D%5Btype%5D=1&amp;t=product-grid</t>
   </si>
   <si>
     <t xml:space="preserve">admin</t>
@@ -124,7 +124,19 @@
     <t xml:space="preserve">UNASSIGNED PRODUCTS AND ITEMS</t>
   </si>
   <si>
+    <t xml:space="preserve">identifier,PRODUCT_DESCRIPTION,BASE_UOM,UOM_QTY_FACTOR</t>
+  </si>
+  <si>
     <t xml:space="preserve">i=1&amp;p=25&amp;s%5Bupdated%5D=1&amp;f%5Bscope%5D%5Bvalue%5D=PRODUCT_CATALOG&amp;f%5Bcategory%5D%5Bvalue%5D%5BtreeId%5D=1&amp;f%5Bcategory%5D%5Bvalue%5D%5BcategoryId%5D=-1&amp;f%5Bcategory%5D%5Btype%5D=1&amp;t=product-grid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Products - COVID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WHO_COVID19_ITEM_CODE,PRODUCT_DESCRIPTION,complete_variant_products,price_reference</t>
+  </si>
+  <si>
+    <t xml:space="preserve">i=1&amp;p=25&amp;s%5BWHO_COVID19_ITEM_CODE%5D=-1&amp;f%5Bscope%5D%5Bvalue%5D=PRODUCT_CATALOG&amp;f%5Bcategory%5D%5Bvalue%5D%5BtreeId%5D=431&amp;f%5Bcategory%5D%5Bvalue%5D%5BcategoryId%5D=0&amp;f%5Bcategory%5D%5Btype%5D=1&amp;t=product-grid</t>
   </si>
 </sst>
 </file>
@@ -139,7 +151,7 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
@@ -226,19 +238,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.6518518518518"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.0222222222222"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.4962962962963"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="110.877777777778"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.44814814814815"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.5"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -426,25 +434,45 @@
         <v>33</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F10" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" s="1" t="s">
         <v>11</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>